<commit_message>
for updated path data
</commit_message>
<xml_diff>
--- a/files/data.xlsx
+++ b/files/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\99gro\Documents\GitHub\Study-of-Emulsion-scattering\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F37658A-D55B-40F8-9F47-E0B724E9672B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEA06E7-0007-4183-9B8A-565E633003B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19599,10 +19599,13 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>